<commit_message>
Atualização da calculadora financeira para v1
</commit_message>
<xml_diff>
--- a/GuilhermeToledo/SimuladorFinanceiro_v0.xlsx
+++ b/GuilhermeToledo/SimuladorFinanceiro_v0.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{071F8D49-B9DE-41ED-A189-BC034C57DE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76DA37-AE53-42E6-AFF1-46FDB6BE44D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EF024B9-F251-4A5D-B513-02DE12B0E257}"/>
   </bookViews>
   <sheets>
     <sheet name="calc v1" sheetId="1" r:id="rId1"/>
     <sheet name="racional pré def" sheetId="2" r:id="rId2"/>
-    <sheet name="draft" sheetId="3" r:id="rId3"/>
+    <sheet name="notas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>metragem área protegida</t>
   </si>
@@ -179,14 +179,73 @@
   </si>
   <si>
     <t>7000 litros gastos em uma área de 24000 m²</t>
+  </si>
+  <si>
+    <t>50 bombeiros para uma área de 50000m²</t>
+  </si>
+  <si>
+    <t>https://sagresonline.com.br/saiba-quanto-custa-tratar-1-litro-de-agua/#:~:text=J%C3%A1%20para%20a%20categoria%20Residencial,e%20distribui%C3%A7%C3%A3o%20da%20%C3%A1gua%20tratada.</t>
+  </si>
+  <si>
+    <t>Para a categoria residencial normal, o custo do metro cúbico de água é de 4.84.</t>
+  </si>
+  <si>
+    <t>litro</t>
+  </si>
+  <si>
+    <t>bombeiros por 10000 m²</t>
+  </si>
+  <si>
+    <t>hora/bombeiro</t>
+  </si>
+  <si>
+    <t>hora/voo</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>litros/m²</t>
+  </si>
+  <si>
+    <t>minutos</t>
+  </si>
+  <si>
+    <t>litros</t>
+  </si>
+  <si>
+    <t>reais</t>
+  </si>
+  <si>
+    <t>avião</t>
+  </si>
+  <si>
+    <t>sim/não</t>
+  </si>
+  <si>
+    <t>bombeiros</t>
+  </si>
+  <si>
+    <t>tempo médio para extinção do incêndio</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-[$R$-416]\ * #,##0.0000_-;\-[$R$-416]\ * #,##0.0000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -234,16 +293,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -253,6 +309,23 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -588,172 +661,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC4B103-E629-498B-A31B-B855ECF12348}">
-  <dimension ref="A6:K32"/>
+  <dimension ref="A6:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="3" t="s">
+      <c r="H10" s="1">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1">
+        <v>180</v>
+      </c>
+      <c r="I11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12">
+        <f>'racional pré def'!K14</f>
+        <v>1.25</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="1" t="s">
+      <c r="H15" s="12">
+        <f>'racional pré def'!K9</f>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="1" t="s">
+      <c r="H16" s="14">
+        <f>'racional pré def'!K10</f>
+        <v>4.8399999999999997E-3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="1" t="s">
+      <c r="H17" s="13">
+        <f>10*(H7/'racional pré def'!K11)</f>
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H18" s="6">
         <f>'racional pré def'!K12</f>
         <v>66.997249999999994</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="1" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="7">
-        <f>'racional pré def'!K13</f>
+      <c r="H20" s="6">
+        <f>IF(H19 = "sim",'racional pré def'!K13,0)</f>
         <v>14047.619047619048</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="1" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="1" t="s">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="3" t="s">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G27" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="3" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="1" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="H29" s="9">
+        <f>IF((H9*60)+(H11*60)*H14&gt;H7,H7,(H9*60)+(H11*60)*H14)</f>
+        <v>17100</v>
+      </c>
+      <c r="I29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="9">
+        <f>IF((H10*60)+(H11*60)*H14&gt;H7,H7,(H10*60)+(H11*60)*H14)</f>
+        <v>15300</v>
+      </c>
+      <c r="K29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="H30" s="6">
+        <f>H18*H17*((H9+H11)/60)</f>
+        <v>8039.6699999999992</v>
+      </c>
+      <c r="J30" s="5">
+        <f>H18*H17*((H10+H11)/60)</f>
+        <v>7034.7112499999994</v>
+      </c>
+      <c r="L30" s="5">
+        <f>H30-J30</f>
+        <v>1004.9587499999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="1" t="s">
+      <c r="H31" s="6">
+        <f>H15*H29*H16</f>
+        <v>283.76228571428567</v>
+      </c>
+      <c r="J31" s="5">
+        <f>H15*J29*H16</f>
+        <v>253.89257142857142</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" ref="L31:L32" si="0">H31-J31</f>
+        <v>29.869714285714252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="3" t="s">
+      <c r="H32" s="6">
+        <f>H20*((H9+H11)/60)</f>
+        <v>56190.476190476191</v>
+      </c>
+      <c r="J32" s="5">
+        <f>H20*((H10+H11)/60)</f>
+        <v>49166.666666666664</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="0"/>
+        <v>7023.8095238095266</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" s="15">
+        <f>SUM(H30:H32)</f>
+        <v>64513.908476190474</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="15">
+        <f>SUM(J30:J32)</f>
+        <v>56455.270488095237</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="15">
+        <f>SUM(L30:L32)</f>
+        <v>8058.6379880952409</v>
+      </c>
+    </row>
+    <row r="34" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
+      <c r="H34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="3"/>
+      <c r="H35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G36" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G32" s="3" t="s">
+    <row r="37" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G38" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -768,13 +992,13 @@
   <dimension ref="G8:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="11" max="11" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="7:16" x14ac:dyDescent="0.25">
@@ -784,7 +1008,7 @@
       <c r="J8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -792,15 +1016,18 @@
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>45</v>
       </c>
       <c r="J9" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <f>24000/7000</f>
         <v>3.4285714285714284</v>
+      </c>
+      <c r="L9" t="s">
+        <v>55</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>6</v>
@@ -810,6 +1037,18 @@
       <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="10">
+        <v>4.8399999999999997E-3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
       <c r="P10" s="1" t="s">
         <v>7</v>
       </c>
@@ -818,6 +1057,18 @@
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="11">
+        <v>10000</v>
+      </c>
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
       <c r="P11" s="1" t="s">
         <v>8</v>
       </c>
@@ -826,15 +1077,18 @@
       <c r="G12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J12" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <f>2679.89/40</f>
         <v>66.997249999999994</v>
+      </c>
+      <c r="L12" t="s">
+        <v>52</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>9</v>
@@ -844,15 +1098,18 @@
       <c r="G13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <f>(5900000/420)</f>
         <v>14047.619047619048</v>
+      </c>
+      <c r="L13" t="s">
+        <v>53</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>19</v>
@@ -862,14 +1119,17 @@
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="J14" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="9">
-        <v>0.5</v>
+      <c r="K14" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="L14" t="s">
+        <v>54</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>10</v>
@@ -881,9 +1141,11 @@
     <hyperlink ref="I14" r:id="rId2" xr:uid="{A84EB857-86FE-42A6-B4A7-E9AA64DAD431}"/>
     <hyperlink ref="I12" r:id="rId3" xr:uid="{1EEE96AA-AF67-4757-B12C-AA1A4E14C161}"/>
     <hyperlink ref="I9" r:id="rId4" xr:uid="{77615B53-3C9F-4821-BD90-7EFF67F5EB92}"/>
+    <hyperlink ref="I11" r:id="rId5" xr:uid="{CC2BB99F-7392-4F66-98C4-F08D091FABE5}"/>
+    <hyperlink ref="I10" r:id="rId6" location=":~:text=J%C3%A1%20para%20a%20categoria%20Residencial,e%20distribui%C3%A7%C3%A3o%20da%20%C3%A1gua%20tratada." xr:uid="{AA5436D9-D730-4003-ACE9-9F26FA66A327}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -892,13 +1154,13 @@
   <dimension ref="G10:G18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="10" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -913,7 +1175,7 @@
       </c>
     </row>
     <row r="14" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -923,7 +1185,7 @@
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>